<commit_message>
Update new filtering draft
</commit_message>
<xml_diff>
--- a/rep_dif_examp_new.xlsx
+++ b/rep_dif_examp_new.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\volume1\ido\BN-SCRIPTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DCC4F9-9109-410C-B0C6-E8D8B626EFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856CD4C4-9538-49EB-9530-49767682F588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{76682717-D6EA-44EF-BD4B-1FC7EB1EF8C9}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>replicate1</t>
   </si>
@@ -59,9 +59,6 @@
     <t>keep</t>
   </si>
   <si>
-    <t>x=&gt;0.8</t>
-  </si>
-  <si>
     <t>0.5&lt;=x&lt;0.8</t>
   </si>
   <si>
@@ -74,21 +71,12 @@
     <t>x=&gt;0.5</t>
   </si>
   <si>
-    <t>d=&gt;0.1</t>
-  </si>
-  <si>
-    <t>d&lt;0.1</t>
-  </si>
-  <si>
     <t>USECASE</t>
   </si>
   <si>
     <t>all</t>
   </si>
   <si>
-    <t>BN_INPUT</t>
-  </si>
-  <si>
     <t>rep1</t>
   </si>
   <si>
@@ -101,9 +89,6 @@
     <t>d&lt;0.3</t>
   </si>
   <si>
-    <t>d=&gt;0.3</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -120,6 +105,24 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>cov&lt;100</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>f&lt;0.01</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>f_tot</t>
+  </si>
+  <si>
+    <t>f2</t>
   </si>
 </sst>
 </file>
@@ -200,23 +203,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,305 +535,273 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2B8186-5620-4EA5-872B-5C7D80C20DDC}">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.26953125" style="4"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.26953125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E6" s="1"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.45</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="B10" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="6" t="s">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5">
+        <v>0.76</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="6" t="s">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="6">
-        <v>1</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0.45</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="6">
-        <v>0.45</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="8">
-        <v>0.3</v>
-      </c>
-      <c r="C13" s="8">
-        <v>0.15</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="8">
+      <c r="B14" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6">
         <v>0.1</v>
       </c>
-      <c r="C14" s="8">
-        <v>0.5</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="C16" s="6">
-        <v>0.76</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="8">
-        <v>0.7</v>
-      </c>
-      <c r="C17" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="D17" s="8" t="s">
+      <c r="E14" s="6"/>
+      <c r="F14" s="6" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>